<commit_message>
Fertig zum Korrekturlesen. Nur noch die Grafiken müssen verbessert und mit einer Beschriftung versehen werden.
</commit_message>
<xml_diff>
--- a/v308/md_helmholtzspule_12cm.xlsx
+++ b/v308/md_helmholtzspule_12cm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a403027534f5acd6/Uni/Physik/Grundpraktikum/Protokolle/v308/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d17f193ba4c0880f/Desktop/Praktikumsberichte/grundpraktikum/v308/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="8_{A49994F7-4605-4E57-9AB8-204E82F0C45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FB35699-F1B6-49BC-8575-7DCB61C930A9}"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C16:C18"/>
+      <selection activeCell="E21" sqref="E21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>